<commit_message>
Commitimg code on 20 March
</commit_message>
<xml_diff>
--- a/Auto-IT/Bulk-Provider-Stable.xlsx
+++ b/Auto-IT/Bulk-Provider-Stable.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\Desktop\BulkUpload\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786445EF-9473-424C-88A3-3DB7C3B0F1F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E9F23DFC-62F0-4F11-A919-B58E4F6C0873}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13510" windowHeight="1950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -935,17 +931,17 @@
     <t>0001</t>
   </si>
   <si>
-    <t>simba-01</t>
-  </si>
-  <si>
-    <t>simba-01@gmail.com</t>
+    <t>simbaprovider-01</t>
+  </si>
+  <si>
+    <t>simbaprovider-01@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1006,6 +1002,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1039,10 +1043,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1061,8 +1066,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1283,15 +1290,15 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.26953125" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" customWidth="1"/>
@@ -1358,7 +1365,7 @@
       <c r="C2" s="5">
         <v>1234567890</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E2" s="5">

</xml_diff>

<commit_message>
Commit on 28 may
</commit_message>
<xml_diff>
--- a/Auto-IT/Bulk-Provider-Stable.xlsx
+++ b/Auto-IT/Bulk-Provider-Stable.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E9F23DFC-62F0-4F11-A919-B58E4F6C0873}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D4B0A415-7B55-4EAB-B014-70D7FE1371E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13510" windowHeight="1950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13440" windowHeight="5730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1290,7 +1290,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>